<commit_message>
Added description of ferritin variables.
</commit_message>
<xml_diff>
--- a/minimal_input.xlsx
+++ b/minimal_input.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="70">
   <si>
     <t xml:space="preserve">Raw input data</t>
   </si>
@@ -70,6 +70,27 @@
     <t xml:space="preserve">First donation date if the first donation in Progesa (yyyymmdd)</t>
   </si>
   <si>
+    <t xml:space="preserve">FERRITIN_FIRST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">double</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First ferritin (ug/L = ng/mL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FERRITIN_LAST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last ferritin (ug/L = ng/mL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FERRITIN_LAST_DATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date when the last ferritin was measured (yyyymmdd)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Donation</t>
   </si>
   <si>
@@ -112,10 +133,7 @@
     <t xml:space="preserve">DONAT_RESULT_CODE</t>
   </si>
   <si>
-    <t xml:space="preserve">double</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hemoglogin (g/L)</t>
+    <t xml:space="preserve">Hemoglogin (g/dL), for example 14.5</t>
   </si>
   <si>
     <t xml:space="preserve">Variables used in prediction</t>
@@ -221,11 +239,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -249,6 +268,11 @@
       <name val="Verdana"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -293,7 +317,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -303,6 +327,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -323,16 +351,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L19" activeCellId="0" sqref="L19"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.09"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="32.37"/>
@@ -415,84 +443,84 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>6</v>
-      </c>
       <c r="D7" s="0" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="2" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="0" t="s">
         <v>19</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="2" t="s">
-        <v>16</v>
+      <c r="B10" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>10</v>
+        <v>25</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="0" t="s">
         <v>27</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>28</v>
@@ -500,144 +528,144 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="0" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>31</v>
       </c>
+      <c r="D14" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="1" t="s">
+      <c r="B16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="2" t="s">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>53</v>
@@ -645,13 +673,13 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>54</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>55</v>
@@ -659,13 +687,13 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>56</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>57</v>
@@ -673,13 +701,13 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>58</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>59</v>
@@ -687,13 +715,13 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>60</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>61</v>
@@ -701,16 +729,58 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>62</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Clarified the input specification
</commit_message>
<xml_diff>
--- a/minimal_input.xlsx
+++ b/minimal_input.xlsx
@@ -61,7 +61,7 @@
     <t xml:space="preserve">KEY_DONOR_DOB</t>
   </si>
   <si>
-    <t xml:space="preserve">Date of birth (e.g. 19580111)</t>
+    <t xml:space="preserve">Date of birth (e.g. 19580111, yyyymmdd)</t>
   </si>
   <si>
     <t xml:space="preserve">DONOR_DATE_FIRST_DONATION</t>
@@ -76,19 +76,19 @@
     <t xml:space="preserve">double</t>
   </si>
   <si>
-    <t xml:space="preserve">First ferritin (ug/L = ng/mL)</t>
+    <t xml:space="preserve">OPTIONAL, First ferritin (ug/L = ng/mL)</t>
   </si>
   <si>
     <t xml:space="preserve">FERRITIN_LAST</t>
   </si>
   <si>
-    <t xml:space="preserve">Last ferritin (ug/L = ng/mL)</t>
+    <t xml:space="preserve">OPTIONAL, Last ferritin (ug/L = ng/mL)</t>
   </si>
   <si>
     <t xml:space="preserve">FERRITIN_LAST_DATE</t>
   </si>
   <si>
-    <t xml:space="preserve">Date when the last ferritin was measured (yyyymmdd)</t>
+    <t xml:space="preserve">OPTIONAL, Date when the last ferritin was measured (yyyymmdd)</t>
   </si>
   <si>
     <t xml:space="preserve">Donation</t>
@@ -112,13 +112,13 @@
     <t xml:space="preserve">DONAT_STATUS</t>
   </si>
   <si>
-    <t xml:space="preserve">Donation status (- =OK, V=change of the bag), R=donation rejected, E=no donation, *=only registration)</t>
+    <t xml:space="preserve">Donation status (- =OK, V=change of the bag, R=disposable blood unit, E=no donation, D=does not fulfill requirements, …). I only check whether status is equal to ‘-’ or not.</t>
   </si>
   <si>
     <t xml:space="preserve">KEY_DONAT_PHLEB</t>
   </si>
   <si>
-    <t xml:space="preserve">Donation Type (K=Whole Blood, P=Plasmapheresis, T=Trombapheresis)</t>
+    <t xml:space="preserve">Donation Type (K=Whole Blood donation, P=Plasmapheresis, T=Trombapheresis, =No donation, H=Whole blood – not studied,…). I only compare whether PHLEB == or != ‘K’, ‘H’, ‘*’</t>
   </si>
   <si>
     <t xml:space="preserve">DONAT_VOL_DRAWN</t>
@@ -239,7 +239,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -269,11 +269,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -317,7 +312,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -330,41 +325,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.09"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="32.37"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -466,7 +455,7 @@
       <c r="D8" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Clarified the input specification2
</commit_message>
<xml_diff>
--- a/minimal_input.xlsx
+++ b/minimal_input.xlsx
@@ -118,7 +118,7 @@
     <t xml:space="preserve">KEY_DONAT_PHLEB</t>
   </si>
   <si>
-    <t xml:space="preserve">Donation Type (K=Whole Blood donation, P=Plasmapheresis, T=Trombapheresis, =No donation, H=Whole blood – not studied,…). I only compare whether PHLEB == or != ‘K’, ‘H’, ‘*’</t>
+    <t xml:space="preserve">Donation Type (K=Whole Blood donation, P=Plasmapheresis, T=Trombapheresis, *=No donation, H=Whole blood – not studied,…). I only compare whether PHLEB == or != ‘K’, ‘H’, ‘*’</t>
   </si>
   <si>
     <t xml:space="preserve">DONAT_VOL_DRAWN</t>
@@ -345,10 +345,10 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.1"/>

</xml_diff>

<commit_message>
Added sex variable to the preprocessed data
</commit_message>
<xml_diff>
--- a/minimal_input.xlsx
+++ b/minimal_input.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="72">
   <si>
     <t xml:space="preserve">Raw input data</t>
   </si>
@@ -230,6 +230,12 @@
   </si>
   <si>
     <t xml:space="preserve">Time of day when donation was given as hours (e.g. 13:45 = 13.75)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“male” or “female”</t>
   </si>
 </sst>
 </file>
@@ -342,13 +348,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.1"/>
@@ -772,6 +778,20 @@
         <v>69</v>
       </c>
     </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>